<commit_message>
add changes to emails
</commit_message>
<xml_diff>
--- a/SEO/emails.xlsx
+++ b/SEO/emails.xlsx
@@ -46,6 +46,9 @@
     <t xml:space="preserve">DHOqH1hYD46Kqoay</t>
   </si>
   <si>
+    <t xml:space="preserve">Taha@61416867</t>
+  </si>
+  <si>
     <t xml:space="preserve">brian@kst-transportation.com</t>
   </si>
   <si>
@@ -119,9 +122,6 @@
   </si>
   <si>
     <t xml:space="preserve">6gw8bGW7z6rn5E94</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taha@61416867</t>
   </si>
 </sst>
 </file>
@@ -162,12 +162,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -204,7 +210,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -217,6 +223,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -226,6 +236,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFF200"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -234,10 +304,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -278,114 +348,112 @@
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>24</v>
+      <c r="A12" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>29</v>
+      <c r="A14" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>31</v>
+      <c r="A15" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A18" r:id="rId1" display="Taha@61416867"/>
+    <hyperlink ref="C3" r:id="rId1" display="Taha@61416867"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>